<commit_message>
upload route, sweet alert, client view
</commit_message>
<xml_diff>
--- a/sample_appointment_nas_eligible.xlsx
+++ b/sample_appointment_nas_eligible.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6780"/>
+    <workbookView windowWidth="23040" windowHeight="9264"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
     <t>ClinicDoctorId</t>
   </si>
@@ -39,6 +39,9 @@
   </si>
   <si>
     <t>EmiratesId</t>
+  </si>
+  <si>
+    <t>MemberId</t>
   </si>
   <si>
     <t>MobileCountryCode</t>
@@ -120,7 +123,7 @@
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
-  <fonts count="22">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -130,13 +133,6 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -621,142 +617,143 @@
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="49">
@@ -1104,20 +1101,22 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:N2"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="15.6818181818182" defaultRowHeight="14.25" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="15.6851851851852" defaultRowHeight="14.4" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="15.6818181818182" customWidth="1"/>
-    <col min="2" max="2" width="22.1363636363636" customWidth="1"/>
-    <col min="3" max="16384" width="15.6818181818182" customWidth="1"/>
+    <col min="1" max="1" width="15.6851851851852" customWidth="1"/>
+    <col min="2" max="2" width="22.1388888888889" customWidth="1"/>
+    <col min="3" max="3" width="15.6851851851852" customWidth="1"/>
+    <col min="4" max="4" width="18.1111111111111" customWidth="1"/>
+    <col min="5" max="16384" width="15.6851851851852" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1160,27 +1159,30 @@
       <c r="N1" s="1" t="s">
         <v>13</v>
       </c>
+      <c r="O1" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" t="s">
         <v>18</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="E2" s="2">
+        <v>123456</v>
+      </c>
+      <c r="F2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="3" t="s">
         <v>20</v>
       </c>
       <c r="H2" t="s">
@@ -1201,7 +1203,10 @@
       <c r="M2" t="s">
         <v>26</v>
       </c>
-      <c r="N2" s="3">
+      <c r="N2" t="s">
+        <v>27</v>
+      </c>
+      <c r="O2" s="4">
         <v>45920.6666666667</v>
       </c>
     </row>

</xml_diff>